<commit_message>
fix price calculation for sell
</commit_message>
<xml_diff>
--- a/contracts/amm_pair/ShadeSwapCalculation.xlsx
+++ b/contracts/amm_pair/ShadeSwapCalculation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Polarity\shadeswap\contracts\amm_pair\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A5AD21E-634C-4A98-A128-A1972420C8DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A0F8A77-23EE-40E3-9846-A5CED23B047F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{F880D771-9217-445A-ABFC-C2E7885C4012}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="31">
   <si>
     <t>Snip 20 - SSRT</t>
   </si>
@@ -126,6 +126,9 @@
   </si>
   <si>
     <t>Price Current Formula</t>
+  </si>
+  <si>
+    <t>Snip 20 - SSRT ( 18 decimals)</t>
   </si>
 </sst>
 </file>
@@ -482,15 +485,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49975B13-9A74-4599-A051-59B5C47586E4}">
   <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.85546875" customWidth="1"/>
     <col min="2" max="2" width="30.85546875" customWidth="1"/>
-    <col min="3" max="3" width="21" customWidth="1"/>
+    <col min="3" max="3" width="27" customWidth="1"/>
     <col min="4" max="5" width="19.28515625" customWidth="1"/>
     <col min="6" max="6" width="18" customWidth="1"/>
     <col min="7" max="7" width="12.42578125" customWidth="1"/>
@@ -540,17 +543,17 @@
         <v>10000000000</v>
       </c>
       <c r="C2" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="D2">
-        <v>100000000</v>
+        <v>100</v>
       </c>
       <c r="E2" t="s">
         <v>9</v>
       </c>
       <c r="F2">
         <f xml:space="preserve"> INT((B2 * D2) / (A2 + D2))</f>
-        <v>99009900</v>
+        <v>99</v>
       </c>
       <c r="G2">
         <f>IF(F2-((B2*D2)/A2)=0,F2-((B2*D2)/A2),0)</f>
@@ -558,17 +561,17 @@
       </c>
       <c r="J2">
         <f>F2/D2</f>
-        <v>0.99009899999999995</v>
+        <v>0.99</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3">
         <f>A2 + D2</f>
-        <v>10100000000</v>
+        <v>10000000100</v>
       </c>
       <c r="B3">
         <f>B2-F2</f>
-        <v>9900990100</v>
+        <v>9999999901</v>
       </c>
       <c r="C3" t="s">
         <v>0</v>
@@ -595,11 +598,11 @@
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
         <f>A3+D3</f>
-        <v>10100000050</v>
+        <v>10000000150</v>
       </c>
       <c r="B4">
         <f>B3-F3</f>
-        <v>9900990051</v>
+        <v>9999999852</v>
       </c>
       <c r="C4" t="s">
         <v>1</v>
@@ -612,25 +615,25 @@
       </c>
       <c r="F4">
         <f xml:space="preserve"> INT((A4 * D4) / (B4 + D4))</f>
-        <v>2550</v>
+        <v>2499</v>
       </c>
       <c r="G4">
         <f>IF(F4-((A4*D4)/B4)=0,F4-((A4*D4)/B4),0)</f>
         <v>0</v>
       </c>
       <c r="J4">
-        <f>F4/D4</f>
-        <v>1.02</v>
+        <f>1/ (F4/D4)</f>
+        <v>1.0004001600640255</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5">
         <f>A4-F4</f>
-        <v>10099997500</v>
+        <v>9999997651</v>
       </c>
       <c r="B5">
         <f>B4+D4</f>
-        <v>9900992551</v>
+        <v>10000002352</v>
       </c>
       <c r="C5" t="s">
         <v>1</v>
@@ -643,25 +646,25 @@
       </c>
       <c r="F5">
         <f xml:space="preserve"> INT((A5 * D5) / (B5 + D5))</f>
-        <v>37233</v>
+        <v>36499</v>
       </c>
       <c r="G5">
         <f>IF(F5-((B5*D5)/A5)=0,F5-((B5*D5)/A5),0)</f>
         <v>0</v>
       </c>
       <c r="J5">
-        <f>F5/D5</f>
-        <v>1.0200821917808218</v>
+        <f>1 / (F5/D5)</f>
+        <v>1.0000273980109045</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6">
         <f>A5-F5</f>
-        <v>10099960267</v>
+        <v>9999961152</v>
       </c>
       <c r="B6">
         <f>B5+D5</f>
-        <v>9901029051</v>
+        <v>10000038852</v>
       </c>
       <c r="C6" t="s">
         <v>0</v>
@@ -674,7 +677,7 @@
       </c>
       <c r="F6">
         <f xml:space="preserve"> INT((B6 * D6) / (A6 + D6))</f>
-        <v>24507</v>
+        <v>25000</v>
       </c>
       <c r="G6">
         <f>IF(F6-((B6*D6)/A6)=0,F6-((B6*D6)/A6),0)</f>
@@ -682,17 +685,17 @@
       </c>
       <c r="J6">
         <f>F6/D6</f>
-        <v>0.98028000000000004</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7">
         <f>A6+D6</f>
-        <v>10099985267</v>
+        <v>9999986152</v>
       </c>
       <c r="B7">
         <f>B6-F6</f>
-        <v>9901004544</v>
+        <v>10000013852</v>
       </c>
     </row>
   </sheetData>
@@ -705,7 +708,7 @@
   <dimension ref="A1:N6"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -722,7 +725,7 @@
     <col min="10" max="10" width="16.5703125" style="1" customWidth="1"/>
     <col min="11" max="11" width="13.85546875" style="1" customWidth="1"/>
     <col min="12" max="12" width="12.85546875" style="1" customWidth="1"/>
-    <col min="13" max="13" width="12.5703125" style="1" customWidth="1"/>
+    <col min="13" max="13" width="15.42578125" style="1" customWidth="1"/>
     <col min="14" max="14" width="17.28515625" style="1" customWidth="1"/>
     <col min="15" max="16384" width="9.140625" style="1"/>
   </cols>

</xml_diff>

<commit_message>
add staking calculation into excel.
</commit_message>
<xml_diff>
--- a/contracts/amm_pair/ShadeSwapCalculation.xlsx
+++ b/contracts/amm_pair/ShadeSwapCalculation.xlsx
@@ -5,16 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Polarity\shadeswap\contracts\amm_pair\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\shadeswap\contracts\amm_pair\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A0F8A77-23EE-40E3-9846-A5CED23B047F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{786E44CF-9F76-424E-8CF0-5DADF0B532E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{F880D771-9217-445A-ABFC-C2E7885C4012}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{F880D771-9217-445A-ABFC-C2E7885C4012}"/>
   </bookViews>
   <sheets>
     <sheet name="CalculationAmountAndPrice" sheetId="1" r:id="rId1"/>
     <sheet name="CalculationLiquidity" sheetId="2" r:id="rId2"/>
+    <sheet name="Staking" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="45">
   <si>
     <t>Snip 20 - SSRT</t>
   </si>
@@ -129,13 +130,55 @@
   </si>
   <si>
     <t>Snip 20 - SSRT ( 18 decimals)</t>
+  </si>
+  <si>
+    <t>LP Token</t>
+  </si>
+  <si>
+    <t>Denominator</t>
+  </si>
+  <si>
+    <t>Stakers</t>
+  </si>
+  <si>
+    <t>Staker A</t>
+  </si>
+  <si>
+    <t>Staker C</t>
+  </si>
+  <si>
+    <t>Staker B</t>
+  </si>
+  <si>
+    <t>Total LP</t>
+  </si>
+  <si>
+    <t>Last Claimable Block Height</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NextClaim Time </t>
+  </si>
+  <si>
+    <t>Claimable Reward</t>
+  </si>
+  <si>
+    <t xml:space="preserve">% Staking </t>
+  </si>
+  <si>
+    <t>Reward Amount</t>
+  </si>
+  <si>
+    <t>Last Time - Current Time in Mils</t>
+  </si>
+  <si>
+    <t>Total Available Reward</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -143,16 +186,29 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -160,17 +216,35 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Check Cell" xfId="1" builtinId="23"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -485,8 +559,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49975B13-9A74-4599-A051-59B5C47586E4}">
   <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -708,7 +782,7 @@
   <dimension ref="A1:N6"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -991,4 +1065,189 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A91B3C8E-34C3-431A-933C-361E4F00399E}">
+  <dimension ref="A1:I7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17" customWidth="1"/>
+    <col min="2" max="3" width="28.5703125" customWidth="1"/>
+    <col min="4" max="4" width="35.42578125" customWidth="1"/>
+    <col min="5" max="5" width="21.5703125" customWidth="1"/>
+    <col min="6" max="6" width="31.42578125" customWidth="1"/>
+    <col min="7" max="8" width="21.5703125" customWidth="1"/>
+    <col min="9" max="9" width="23" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H1" t="s">
+        <v>44</v>
+      </c>
+      <c r="I1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2">
+        <v>100000</v>
+      </c>
+      <c r="C2">
+        <f>B2/$B5</f>
+        <v>2.1919729948927029E-5</v>
+      </c>
+      <c r="D2">
+        <v>1656480000</v>
+      </c>
+      <c r="E2">
+        <v>1656480524</v>
+      </c>
+      <c r="F2">
+        <f>E2-D2</f>
+        <v>524</v>
+      </c>
+      <c r="G2">
+        <f>24*60*60*1000</f>
+        <v>86400000</v>
+      </c>
+      <c r="H2">
+        <f>(B6/G2) *F2</f>
+        <v>20923611.111111112</v>
+      </c>
+      <c r="I2">
+        <f>INT(H2*C2)</f>
+        <v>458</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3">
+        <v>2000000</v>
+      </c>
+      <c r="C3">
+        <f>B3/$B5</f>
+        <v>4.3839459897854059E-4</v>
+      </c>
+      <c r="D3">
+        <v>1656480000</v>
+      </c>
+      <c r="E3">
+        <v>1656480524</v>
+      </c>
+      <c r="F3">
+        <f t="shared" ref="F3:F4" si="0">E3-D3</f>
+        <v>524</v>
+      </c>
+      <c r="G3">
+        <f t="shared" ref="G3:G4" si="1">24*60*60*1000</f>
+        <v>86400000</v>
+      </c>
+      <c r="H3">
+        <f>(B6/G3) *F3</f>
+        <v>20923611.111111112</v>
+      </c>
+      <c r="I3">
+        <f t="shared" ref="I3:I4" si="2">INT(H3*C3)</f>
+        <v>9172</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4">
+        <v>4560000000</v>
+      </c>
+      <c r="C4">
+        <f>B4/$B5</f>
+        <v>0.99953968567107254</v>
+      </c>
+      <c r="D4">
+        <v>1656480000</v>
+      </c>
+      <c r="E4">
+        <v>1656480524</v>
+      </c>
+      <c r="F4">
+        <f t="shared" si="0"/>
+        <v>524</v>
+      </c>
+      <c r="G4">
+        <f t="shared" si="1"/>
+        <v>86400000</v>
+      </c>
+      <c r="H4">
+        <f>(B6/G4) *F4</f>
+        <v>20923611.111111112</v>
+      </c>
+      <c r="I4">
+        <f t="shared" si="2"/>
+        <v>20913979</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5">
+        <f xml:space="preserve"> SUM(B2:B4)</f>
+        <v>4562100000</v>
+      </c>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+    </row>
+    <row r="6" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6">
+        <v>3450000000000</v>
+      </c>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+    </row>
+    <row r="7" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add remove liquidity via unstake
</commit_message>
<xml_diff>
--- a/contracts/amm_pair/ShadeSwapCalculation.xlsx
+++ b/contracts/amm_pair/ShadeSwapCalculation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Polarity\shadeswap\contracts\amm_pair\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\shadeswap\contracts\amm_pair\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{696AF456-60E4-42FE-A682-54CD3BDCE622}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E50774B9-B103-4095-8574-E2C95082C15D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{F880D771-9217-445A-ABFC-C2E7885C4012}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{F880D771-9217-445A-ABFC-C2E7885C4012}"/>
   </bookViews>
   <sheets>
     <sheet name="CalculationAmountAndPrice" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="49">
   <si>
     <t>Snip 20 - SSRT</t>
   </si>
@@ -181,6 +181,9 @@
   </si>
   <si>
     <t>Deducted Offer Amount</t>
+  </si>
+  <si>
+    <t>Price</t>
   </si>
 </sst>
 </file>
@@ -588,10 +591,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49975B13-9A74-4599-A051-59B5C47586E4}">
-  <dimension ref="A1:M7"/>
+  <dimension ref="A1:N7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -609,7 +612,7 @@
     <col min="14" max="14" width="14.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -649,8 +652,11 @@
       <c r="M1" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N1" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>10000000000</v>
       </c>
@@ -694,8 +700,12 @@
         <f xml:space="preserve"> INT((B2 *L2) / (A2 + L2))</f>
         <v>89</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N2">
+        <f xml:space="preserve"> M2/E2</f>
+        <v>0.89</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3">
         <f>A2 +L2+H2</f>
         <v>10000000098</v>
@@ -720,7 +730,7 @@
         <v>100</v>
       </c>
       <c r="H3">
-        <f t="shared" ref="H3:H6" si="0">INT((F3*E3) /G3)</f>
+        <f>INT((F3*E3) /G3)</f>
         <v>4</v>
       </c>
       <c r="I3">
@@ -730,25 +740,29 @@
         <v>100</v>
       </c>
       <c r="K3">
-        <f t="shared" ref="K3:K6" si="1">INT((E3 *I3)/J3)</f>
+        <f>INT((E3 *I3)/J3)</f>
         <v>1</v>
       </c>
       <c r="L3" s="5">
-        <f t="shared" ref="L3:L6" si="2">E3-H3-K3</f>
+        <f>E3-H3-K3</f>
         <v>45</v>
       </c>
       <c r="M3">
-        <f t="shared" ref="M3:M6" si="3" xml:space="preserve"> INT((B3 *L3) / (A3 + L3))</f>
+        <f xml:space="preserve"> INT((B3 *L3) / (A3 + L3))</f>
         <v>44</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N3">
+        <f xml:space="preserve"> M3/E3</f>
+        <v>0.88</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4">
-        <f t="shared" ref="A4:A7" si="4">A3 +L3+H3</f>
+        <f>A3 +L3+H3</f>
         <v>10000000147</v>
       </c>
       <c r="B4">
-        <f t="shared" ref="B4:B7" si="5">B3-M3</f>
+        <f>B3-M3</f>
         <v>9999999867</v>
       </c>
       <c r="C4" t="s">
@@ -767,7 +781,7 @@
         <v>100</v>
       </c>
       <c r="H4">
-        <f t="shared" si="0"/>
+        <f>INT((F4*E4) /G4)</f>
         <v>200</v>
       </c>
       <c r="I4">
@@ -777,26 +791,30 @@
         <v>100</v>
       </c>
       <c r="K4">
-        <f t="shared" si="1"/>
+        <f>INT((E4 *I4)/J4)</f>
         <v>50</v>
       </c>
       <c r="L4" s="5">
-        <f t="shared" si="2"/>
+        <f>E4-H4-K4</f>
         <v>2250</v>
       </c>
       <c r="M4">
-        <f t="shared" si="3"/>
+        <f xml:space="preserve"> INT((B4 *L4) / (A4 + L4))</f>
         <v>2249</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N4">
+        <f>(M4/E4) /1</f>
+        <v>0.89959999999999996</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5">
-        <f t="shared" si="4"/>
-        <v>10000002597</v>
+        <f>A4 -M4</f>
+        <v>9999997898</v>
       </c>
       <c r="B5">
-        <f t="shared" si="5"/>
-        <v>9999997618</v>
+        <f>B4 +M4+H4</f>
+        <v>10000002316</v>
       </c>
       <c r="C5" t="s">
         <v>1</v>
@@ -814,7 +832,7 @@
         <v>100</v>
       </c>
       <c r="H5">
-        <f t="shared" si="0"/>
+        <f>INT((F5*E5) /G5)</f>
         <v>2920</v>
       </c>
       <c r="I5">
@@ -824,26 +842,30 @@
         <v>100</v>
       </c>
       <c r="K5">
-        <f t="shared" si="1"/>
+        <f>INT((E5 *I5)/J5)</f>
         <v>730</v>
       </c>
       <c r="L5" s="5">
-        <f t="shared" si="2"/>
+        <f>E5-H5-K5</f>
         <v>32850</v>
       </c>
       <c r="M5">
-        <f t="shared" si="3"/>
+        <f xml:space="preserve"> INT((B5 *L5) / (A5 + L5))</f>
         <v>32849</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N5">
+        <f>(M5/E5) /1</f>
+        <v>0.89997260273972601</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6">
-        <f t="shared" si="4"/>
-        <v>10000038367</v>
+        <f>A5 -M5</f>
+        <v>9999965049</v>
       </c>
       <c r="B6">
-        <f t="shared" si="5"/>
-        <v>9999964769</v>
+        <f>B5 + L5+H5</f>
+        <v>10000038086</v>
       </c>
       <c r="C6" t="s">
         <v>0</v>
@@ -861,7 +883,7 @@
         <v>100</v>
       </c>
       <c r="H6">
-        <f t="shared" si="0"/>
+        <f>INT((F6*E6) /G6)</f>
         <v>2000</v>
       </c>
       <c r="I6">
@@ -871,30 +893,35 @@
         <v>100</v>
       </c>
       <c r="K6">
-        <f t="shared" si="1"/>
+        <f>INT((E6 *I6)/J6)</f>
         <v>500</v>
       </c>
       <c r="L6" s="5">
-        <f t="shared" si="2"/>
+        <f>E6-H6-K6</f>
         <v>22500</v>
       </c>
       <c r="M6">
-        <f t="shared" si="3"/>
-        <v>22499</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+        <f xml:space="preserve"> INT((B6 *L6) / (A6 + L6))</f>
+        <v>22500</v>
+      </c>
+      <c r="N6">
+        <f>M6/E6</f>
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7">
-        <f t="shared" si="4"/>
-        <v>10000062867</v>
+        <f>A6 +L6+H6</f>
+        <v>9999989549</v>
       </c>
       <c r="B7">
-        <f t="shared" si="5"/>
-        <v>9999942270</v>
+        <f>B6-M6</f>
+        <v>10000015586</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -903,7 +930,7 @@
   <dimension ref="A1:N6"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1061,7 +1088,7 @@
         <v>0</v>
       </c>
       <c r="M3" s="1">
-        <f t="shared" ref="M3:M4" si="0">J3+K3+L3</f>
+        <f>J3+K3+L3</f>
         <v>10000000000</v>
       </c>
       <c r="N3" s="1">
@@ -1071,11 +1098,11 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <f t="shared" ref="A4:A5" si="1" xml:space="preserve"> A3 + D3 + F3+H3</f>
+        <f xml:space="preserve"> A3 + D3 + F3+H3</f>
         <v>20000000000</v>
       </c>
       <c r="B4" s="1">
-        <f t="shared" ref="B4:B5" si="2" xml:space="preserve"> B3 + E3+G3+I3</f>
+        <f xml:space="preserve"> B3 + E3+G3+I3</f>
         <v>20000000000</v>
       </c>
       <c r="C4" s="1" t="s">
@@ -1112,7 +1139,7 @@
         <v>10000000</v>
       </c>
       <c r="M4" s="1">
-        <f t="shared" si="0"/>
+        <f>J4+K4+L4</f>
         <v>10000000</v>
       </c>
       <c r="N4" s="1">
@@ -1122,11 +1149,11 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <f t="shared" si="1"/>
+        <f xml:space="preserve"> A4 + D4 + F4+H4</f>
         <v>20010000000</v>
       </c>
       <c r="B5" s="1">
-        <f t="shared" si="2"/>
+        <f xml:space="preserve"> B4 + E4+G4+I4</f>
         <v>20010000000</v>
       </c>
       <c r="C5" s="1" t="s">
@@ -1193,7 +1220,7 @@
   <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1288,11 +1315,11 @@
         <v>1656480524</v>
       </c>
       <c r="F3">
-        <f t="shared" ref="F3:F4" si="0">E3-D3</f>
+        <f>E3-D3</f>
         <v>524</v>
       </c>
       <c r="G3">
-        <f t="shared" ref="G3:G4" si="1">24*60*60*1000</f>
+        <f>24*60*60*1000</f>
         <v>86400000</v>
       </c>
       <c r="H3">
@@ -1300,7 +1327,7 @@
         <v>20923611.111111112</v>
       </c>
       <c r="I3">
-        <f t="shared" ref="I3:I4" si="2">INT(H3*C3)</f>
+        <f>INT(H3*C3)</f>
         <v>9172</v>
       </c>
     </row>
@@ -1322,11 +1349,11 @@
         <v>1656480524</v>
       </c>
       <c r="F4">
-        <f t="shared" si="0"/>
+        <f>E4-D4</f>
         <v>524</v>
       </c>
       <c r="G4">
-        <f t="shared" si="1"/>
+        <f>24*60*60*1000</f>
         <v>86400000</v>
       </c>
       <c r="H4">
@@ -1334,7 +1361,7 @@
         <v>20923611.111111112</v>
       </c>
       <c r="I4">
-        <f t="shared" si="2"/>
+        <f>INT(H4*C4)</f>
         <v>20913979</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add new lp token calculation
</commit_message>
<xml_diff>
--- a/contracts/amm_pair/ShadeSwapCalculation.xlsx
+++ b/contracts/amm_pair/ShadeSwapCalculation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\shadeswap\contracts\amm_pair\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Polarity\shadeswap\contracts\amm_pair\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E50774B9-B103-4095-8574-E2C95082C15D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F033F9E5-04E4-4296-88FA-693148A82867}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{F880D771-9217-445A-ABFC-C2E7885C4012}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="2" xr2:uid="{F880D771-9217-445A-ABFC-C2E7885C4012}"/>
   </bookViews>
   <sheets>
     <sheet name="CalculationAmountAndPrice" sheetId="1" r:id="rId1"/>
@@ -593,7 +593,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49975B13-9A74-4599-A051-59B5C47586E4}">
   <dimension ref="A1:N7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
@@ -1219,8 +1219,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A91B3C8E-34C3-431A-933C-361E4F00399E}">
   <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1268,11 +1268,11 @@
         <v>31</v>
       </c>
       <c r="B2">
-        <v>100000</v>
+        <v>10000000000</v>
       </c>
       <c r="C2">
         <f>B2/$B5</f>
-        <v>2.1919729948927029E-5</v>
+        <v>0.68671885729982141</v>
       </c>
       <c r="D2">
         <v>1656480000</v>
@@ -1294,7 +1294,7 @@
       </c>
       <c r="I2">
         <f>INT(H2*C2)</f>
-        <v>458</v>
+        <v>14368638</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -1306,7 +1306,7 @@
       </c>
       <c r="C3">
         <f>B3/$B5</f>
-        <v>4.3839459897854059E-4</v>
+        <v>1.373437714599643E-4</v>
       </c>
       <c r="D3">
         <v>1656480000</v>
@@ -1328,7 +1328,7 @@
       </c>
       <c r="I3">
         <f>INT(H3*C3)</f>
-        <v>9172</v>
+        <v>2873</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1340,7 +1340,7 @@
       </c>
       <c r="C4">
         <f>B4/$B5</f>
-        <v>0.99953968567107254</v>
+        <v>0.31314379892871858</v>
       </c>
       <c r="D4">
         <v>1656480000</v>
@@ -1362,7 +1362,7 @@
       </c>
       <c r="I4">
         <f>INT(H4*C4)</f>
-        <v>20913979</v>
+        <v>6552099</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1371,7 +1371,7 @@
       </c>
       <c r="B5">
         <f xml:space="preserve"> SUM(B2:B4)</f>
-        <v>4562100000</v>
+        <v>14562000000</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>

</xml_diff>